<commit_message>
Added a file with a structure for storing the cost of an hour of an employee.
</commit_message>
<xml_diff>
--- a/Parameters/UCosts.xlsx
+++ b/Parameters/UCosts.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380F016B-6D6A-45A2-8D2C-CE987EAE5B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E498BA-B6BD-428B-B1B9-38C4A6FCFE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,15 +29,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>UserName</t>
+    <t>UserCostPodr</t>
   </si>
   <si>
-    <t>Cost</t>
+    <t>CostUserName</t>
   </si>
   <si>
-    <t>UserPodr</t>
+    <t>UserHourCost</t>
+  </si>
+  <si>
+    <t>UserMonthCost</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F53492B-E9B6-44FD-A10D-37455B40CAC6}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -414,209 +417,249 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D24">
     <sortCondition ref="B2:B24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>